<commit_message>
removed the usage of the abstract state for REFPROP in the heat exchanger class, because the initial fluid composition was set wrong. Perhaps a pointer issue? a copy could help? The hex_exc_run script must be modified, the copying is not correct.
</commit_message>
<xml_diff>
--- a/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
+++ b/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atakan\sciebo\Python\carbatpy\carbatpy\src\work_in_progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DB27C1B-17B1-41F0-B24B-2C1BA1DEC5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88242AF-687F-4AF5-BE56-8279C299D7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61650" yWindow="6435" windowWidth="14400" windowHeight="8190" activeTab="2" xr2:uid="{4E6C26D7-6C6E-4333-9A67-A60B9315F33E}"/>
+    <workbookView xWindow="60765" yWindow="3165" windowWidth="14400" windowHeight="8190" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -18,214 +18,200 @@
     <sheet name="Fluid_2" sheetId="3" r:id="rId3"/>
     <sheet name="Problem_description" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
+    <t>variable_name</t>
+  </si>
+  <si>
+    <t>value_1</t>
+  </si>
+  <si>
+    <t>value_2</t>
+  </si>
+  <si>
+    <t>fixed_1</t>
+  </si>
+  <si>
+    <t>fixed_2</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>hex_type</t>
+  </si>
+  <si>
+    <t>counterflow</t>
+  </si>
+  <si>
+    <t>specification</t>
+  </si>
+  <si>
+    <t>shellTube</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>W/ m2 / K</t>
+  </si>
+  <si>
+    <t>tubes</t>
+  </si>
+  <si>
+    <t>d_in</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>wall_thickness</t>
+  </si>
+  <si>
+    <t>cp</t>
+  </si>
+  <si>
+    <t>J/kg/K</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>kg/m3</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>W / m / K</t>
+  </si>
+  <si>
+    <t>thermal_conductivity</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>Fluid_1</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Name of Sheet for the selection of 1 or two fluids,or  value_2: constant or T-slope</t>
+  </si>
+  <si>
+    <t>hex_name</t>
+  </si>
+  <si>
+    <t>condenser0</t>
+  </si>
+  <si>
+    <t>no_points</t>
+  </si>
+  <si>
+    <t>calc_type</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>value_min</t>
+  </si>
+  <si>
+    <t>value_max</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>name_fluid</t>
+  </si>
+  <si>
+    <t>value_choices</t>
+  </si>
+  <si>
     <t>props</t>
   </si>
   <si>
-    <t>tubes</t>
-  </si>
-  <si>
-    <t>d_in</t>
-  </si>
-  <si>
-    <t>length</t>
+    <t>REFPROP</t>
+  </si>
+  <si>
+    <t>number_compounds</t>
   </si>
   <si>
     <t>fl1</t>
   </si>
   <si>
+    <t>Propane</t>
+  </si>
+  <si>
+    <t>mole fraction</t>
+  </si>
+  <si>
     <t>fl2</t>
   </si>
   <si>
+    <t>Pentane</t>
+  </si>
+  <si>
+    <t>T_in</t>
+  </si>
+  <si>
     <t>K</t>
   </si>
   <si>
-    <t>REFPROP</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Propane</t>
-  </si>
-  <si>
-    <t>Pentane</t>
+    <t>p_in</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>m_dot</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>units</t>
   </si>
   <si>
     <t>Water</t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>fixed</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>T_in</t>
-  </si>
-  <si>
-    <t>p_in</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Pa</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>value_1</t>
-  </si>
-  <si>
-    <t>m_dot</t>
-  </si>
-  <si>
-    <t>kg/s</t>
-  </si>
-  <si>
-    <t>counterflow</t>
-  </si>
-  <si>
-    <t>specification</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>W/ m2 / K</t>
-  </si>
-  <si>
-    <t>wall_thickness</t>
-  </si>
-  <si>
-    <t>cp</t>
-  </si>
-  <si>
-    <t>rho</t>
-  </si>
-  <si>
-    <t>material</t>
-  </si>
-  <si>
-    <t>Steel</t>
-  </si>
-  <si>
-    <t>kg/m3</t>
-  </si>
-  <si>
-    <t>J/kg/K</t>
-  </si>
-  <si>
-    <t>value_min</t>
-  </si>
-  <si>
-    <t>value_max</t>
-  </si>
-  <si>
-    <t>name_fluid</t>
-  </si>
-  <si>
-    <t>mole fraction</t>
+    <t>unused</t>
+  </si>
+  <si>
+    <t>calculation_type</t>
   </si>
   <si>
     <t>output</t>
   </si>
   <si>
-    <t>calculation_type</t>
-  </si>
-  <si>
-    <t>W / m / K</t>
-  </si>
-  <si>
-    <t>shellTube</t>
-  </si>
-  <si>
-    <t>hex_type</t>
-  </si>
-  <si>
-    <t>number_compounds</t>
-  </si>
-  <si>
     <t>T_ref</t>
-  </si>
-  <si>
-    <t>option</t>
-  </si>
-  <si>
-    <t>thermal_conductivity</t>
-  </si>
-  <si>
-    <t>variable_name</t>
-  </si>
-  <si>
-    <t>value_2</t>
-  </si>
-  <si>
-    <t>fixed_1</t>
-  </si>
-  <si>
-    <t>fixed_2</t>
-  </si>
-  <si>
-    <t>value_choices</t>
-  </si>
-  <si>
-    <t>unused</t>
-  </si>
-  <si>
-    <t>configuration</t>
-  </si>
-  <si>
-    <t>Fluid_1</t>
-  </si>
-  <si>
-    <t>constant</t>
-  </si>
-  <si>
-    <t>Name of Sheet for the selection of 1 or two fluids,or  value_2: constant or T-slope</t>
-  </si>
-  <si>
-    <t>hex_name</t>
-  </si>
-  <si>
-    <t>condenser0</t>
-  </si>
-  <si>
-    <t>no_points</t>
-  </si>
-  <si>
-    <t>calc_type</t>
-  </si>
-  <si>
-    <t>const</t>
-  </si>
-  <si>
-    <t>units</t>
   </si>
 </sst>
 </file>
@@ -577,7 +563,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E9C067-F795-4212-A253-B3A1494FB4F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -594,49 +580,49 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -645,18 +631,18 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -665,15 +651,15 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>0.01</v>
@@ -682,35 +668,35 @@
         <v>0.08</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1">
         <v>1E-3</v>
@@ -719,18 +705,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>800</v>
@@ -739,18 +725,18 @@
         <v>800</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
         <v>8000</v>
@@ -759,38 +745,38 @@
         <v>8000</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
         <v>16</v>
@@ -799,37 +785,37 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -837,10 +823,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -849,11 +835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01BE42C-B3CE-4C88-976A-3493C0B4F75D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -863,47 +849,47 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -911,10 +897,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -923,21 +909,21 @@
         <v>0.8</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -946,18 +932,18 @@
         <v>0.9</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>350</v>
@@ -969,15 +955,15 @@
         <v>370</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1">
         <v>1000000</v>
@@ -989,15 +975,15 @@
         <v>2000000</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>1.2E-2</v>
@@ -1009,12 +995,12 @@
         <v>0.02</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -1026,11 +1012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1136C784-1A7F-40CC-B5EA-CA25A67293E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1040,47 +1026,47 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1088,7 +1074,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1100,21 +1086,21 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B5">
-        <v>350</v>
+        <v>299</v>
       </c>
       <c r="C5">
         <v>290</v>
@@ -1123,15 +1109,15 @@
         <v>370</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1">
         <v>1000000</v>
@@ -1143,18 +1129,18 @@
         <v>2000000</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B7">
-        <v>1.2E-2</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="C7">
         <v>0.01</v>
@@ -1163,12 +1149,12 @@
         <v>0.02</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>21</v>
@@ -1189,7 +1175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A56B6A2-0CAF-4DED-8F52-E833FCDF80DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1203,53 +1189,53 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>283.14999999999998</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The heat_exc_run_script together with heat_exchanger runs after avoiding to set the fluids to "". Only then the boundary conditions are set correctly. There is something wrong otherwise, but I could not find it.
</commit_message>
<xml_diff>
--- a/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
+++ b/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atakan\sciebo\Python\carbatpy\carbatpy\src\work_in_progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88242AF-687F-4AF5-BE56-8279C299D7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CCAA22-A299-4976-AB9C-AB91617D8A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60765" yWindow="3165" windowWidth="14400" windowHeight="8190" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61770" yWindow="4170" windowWidth="14400" windowHeight="8190" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
   <si>
     <t>variable_name</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>T_ref</t>
+  </si>
+  <si>
+    <t>fl3</t>
+  </si>
+  <si>
+    <t>Butane</t>
   </si>
 </sst>
 </file>
@@ -836,7 +842,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -892,7 +898,7 @@
         <v>45</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
@@ -923,7 +929,7 @@
         <v>49</v>
       </c>
       <c r="B5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -943,66 +949,89 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B6">
-        <v>350</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
-        <v>290</v>
+        <v>0.1</v>
       </c>
       <c r="D6">
-        <v>370</v>
+        <v>0.6</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="C7" s="1">
-        <v>100000</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2000000</v>
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>370</v>
+      </c>
+      <c r="C7">
+        <v>290</v>
+      </c>
+      <c r="D7">
+        <v>370</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C8">
-        <v>0.01</v>
-      </c>
-      <c r="D8">
-        <v>0.02</v>
+        <v>53</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1300000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>0.02</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>21</v>
       </c>
     </row>
@@ -1140,7 +1169,7 @@
         <v>55</v>
       </c>
       <c r="B7">
-        <v>3.2000000000000002E-3</v>
+        <v>9.1999999999999998E-3</v>
       </c>
       <c r="C7">
         <v>0.01</v>

</xml_diff>

<commit_message>
workaround for the refprop-problem: a copy of REFPROP is used to have two independent versions/modules. It now also works with the fluids set to "" after the first call.
</commit_message>
<xml_diff>
--- a/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
+++ b/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atakan\sciebo\Python\carbatpy\carbatpy\src\work_in_progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CCAA22-A299-4976-AB9C-AB91617D8A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0961D095-AFB8-40BF-8C16-673C2359C6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="61770" yWindow="4170" windowWidth="14400" windowHeight="8190" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,7 +845,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -906,7 +906,7 @@
         <v>46</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -929,7 +929,7 @@
         <v>49</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -952,7 +952,7 @@
         <v>63</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C6">
         <v>0.1</v>
@@ -1015,7 +1015,7 @@
         <v>55</v>
       </c>
       <c r="B9">
-        <v>0.01</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="C9">
         <v>0.01</v>

</xml_diff>

<commit_message>
unique variable names introduced for heat-exchanger-result storage in Excel-file
now  "_fl1" or "_fl2" is added to the variable names of the two fluids
</commit_message>
<xml_diff>
--- a/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
+++ b/carbatpy/src/work_in_progress/heat_exchanger_input1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atakan\sciebo\Python\carbatpy\carbatpy\src\work_in_progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0961D095-AFB8-40BF-8C16-673C2359C6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981C0F09-CAB3-4A97-87D7-4B636525EBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61770" yWindow="4170" windowWidth="14400" windowHeight="8190" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60540" yWindow="3240" windowWidth="25860" windowHeight="10710" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -845,7 +845,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -929,7 +929,7 @@
         <v>49</v>
       </c>
       <c r="B5">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -952,7 +952,7 @@
         <v>63</v>
       </c>
       <c r="B6">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="C6">
         <v>0.1</v>

</xml_diff>